<commit_message>
Allowed user to input job to search for, cleaned up the code a bit
</commit_message>
<xml_diff>
--- a/jobs.xlsx
+++ b/jobs.xlsx
@@ -408,12 +408,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,6 +439,11 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>Salary</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>Apply Here</t>
         </is>
       </c>
@@ -446,334 +451,258 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Software Developer</t>
+          <t>Associate Software Developer Apprentice</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Bioviratech</t>
+          <t>Pearson</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>London</t>
+          <t>Remote in London</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0BmXmoSiuR-3iizRQqbT4uBogWdtgOZbaQF9xQI5H_uM3QM3MI7dYoGmzBRSF2ZY-_XMMAiPR6ZgQbGKUchnrnfL-iu1FLR8jbclLo0QzKonyaf4_eJIDF1SPVwPh_dKUy1gT20j3Eal8jeYdQvgFuiVQkScNTWbT1uERAtLaMQvMNkp3THi7YqFa4Pr2UBi_qwfPx4yhaX8muwc3VaOTpI80tek-4IZ7dduQRyS4aSDfoou9aay1uMZuY2OUkp9GHC7lYoXYiVUU3HbEr39nrmBoS8ABW8qiV8aKhg6e7utNXTnqlkmTXiJkRnlVoZ0Xu30hwHL2cW2T_r72FjFY0cAidm9dDORIjyHvbdS76zviNISu5RBSd_U_u7lrl9kaeRfp_pTjy8ZaFQR7Hj1LAQVHqaAMruCJ6ED4uwRqxJPd3d61EhZc5MCPLBXUUw-_7tqyYXNYeGC97Ej1WaTauE1q0V41u8tRoBhkp5F76MyQ==&amp;xkcb=SoAL-_M3cgKcSUA5rj0LbzkdCdPP&amp;p=0&amp;fvj=1&amp;vjs=3</t>
+          <t>£22,000 - £25,000 a year</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>test/rc/clk?jk=002bf4846fcb7d28&amp;fccid=915b1c0ee87e5e8a&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Full Stack Software Developer</t>
+          <t>Software Junior Developer Apprentice</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>TryHackMe</t>
+          <t>QA Apprenticeships</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Remote in London</t>
+          <t>London EC2M</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0CVjb1APgAsEHI3OPdF_Fe_zurvzy-DduGi_D65iV7dqcrCy26bXX2QLRz0gyLSGLEdtdxAhgynkzHJDpTIpYeNxBmWObS2Vx3Dezno7GnIyx0znvMDK_vGUs4UvCBabstGwaaY0cMLajYb24hXGq4hXiVPPT8BTb7uY_IX7Ns0P-IbrO_UL7aqOUGZakz8FOhO5RXKESXWXgzb-4CRArFlL30MWgf9pSeptMLGSnkdxBiBek_WoX_d8hA_iQmYdohXf-5fGHqqv-x4qVz1t7SJK4KM6pEb1aIImU8r6yym8FqofvNZ9U5DW-y0dYW-b0E1IoJpzvdMlVJ0ZeGJw1jVLJbbF4eUgfidN5xN1zmN0kBLw87Pr-uFsPBnxiAUQ30bk7ORcluYuJ3mBZ7TvR3LhNArXMl02P9YW-x2haIJchQm57MF5jY_8ANWNJJP0nN-aFkXM-tzJCFWuvh6eWhHLxlxAf4JbdjGX8lr0r0UxeaYL3SwU28s&amp;xkcb=SoD6-_M3cgKcSUg5rj0KbzkdCdPP&amp;p=1&amp;fvj=1&amp;vjs=3</t>
+          <t>£25,000 - £30,000 a year</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>test/pagead/clk?mo=r&amp;ad=-6NYlbfkN0CXy9_N1TLC2ejqyTX_V4eQ4PmQ2039NyFlBjhJ2joCdiLJ2guK6p6gDxKa49r6zxjCTAdQ1uM6iXGzvNU-Yc7zz3hcZmLelAG_vJQZlpFH00o1s04wldLCcuG3xoLJUNvg5I_mfxXCc_PV8WtCkXK1fUnA5Ex_hentUerjmxq2xmbvt24wPEOhAt-4w0krKuY-5OC1YS1GG8ekoDS0pUvI9LB72Jbk-px0W1IHgYf2nnyKhygMNemCiNhxr6fwaA69LYKM45kVJZ45QUPOiGNyc0P3Bxd6RuqbJbi1M5HxoOAYwevuidoX8c1_R9ukVmVc48n3TDL0IMNmdc4N9vufm8IkpwGJZqwDrWj10JKh0p8tBBcpC2W2oaGSpfeBrtAhQTcwhgXFO7H2sMiaJ1SHql9Cg8qrSW8wW3OuRbyC9D1g_j8Y575urpomtH8gy-_h4m2_9wVcvLHsCr4CADU40sJAalV6IQXDY7FBh-hzlTmEi_TLXsHTyH5gt7ZglxClV7w7I8qPjXY0KCA00rNqdbwUZLvf0lypRVaTQDJk9tmrkLwVsDtJ&amp;xkcb=SoDK-_M3c1NbXUwHsp0LbzkdCdPP&amp;p=4&amp;fvj=0&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Front End Developer</t>
+          <t>We are recruiting an Apprentice Software Developer</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Civica</t>
+          <t>thecitysecret</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>London</t>
+          <t>Richmond</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0DG4ntHtB_rMsnfhgmnSvK2brktLme1L4SiDeJjQ-izrVOLqRJ5-yjEhSyAj73O13THNhMbzyKKBJ7Ay0Ed9-3iHsIQ0gjp6en0OgexjNBO7Qvn_iB2d57mXL3Spk9_NOEh1q-9CHWnfe1KYS1-cf9EoVzXYzkkRBe0NVc99GY1QbDiAivLqejpbBZyzwxWVyMeSXYUcP8QsqK0q4tkc_skWIZjOHSjs3oHSkM0daP5Y3zCIhgMWtI8xOvIe1Ie96kgW-CE3atEJXqA9eD3_ckjxWOalzmxoTusBxVho2Y4xMPjh5sGgnlanwU-GjtpQQ3XynTza_Ua8Qi330bSkuZwYZ9Lcim-qyOydnUXCEGIBCTPHV2kCRk1Iu2iarCEJs5jTrRe7IpMmKqMxHJXHTFGX4wb2pRpnfVnHFIaGGkZ2EXdke9pqZyJe4vqfAGHO1UEoToIykev9AB2r-TNaWeMlRjWTqXqyJlFB_N3kWqwn5XMo9HHiAeDZq4y98a6-VrQISDEviMWKYkxvF3SwHFfvi3LQk3KCiJ_uIArDis7xI6EXfy3wc_RGhxfv57BRy8JYQefSF7YcUV8Ww5rXEfkiqNCINorWV0Qoveo8NIi1ALC7xx2c6FPn_iy7FGixhbN50vzboVd4Mz2kMeCdjQrJ7bTmnPm6AqBQPzyoe_bWCQbh3vyJD6uxK8S9hvq0ovUycRl9Ty_adij2FifSa1_CTKR2jMgG9AS9ymuoocMfM0G5CRkhlcKu1h_z8LkyGwGWZPoQrWVU3tbGUkFz52WpPXJGW-iGY0Ise7zRbuqMtJfJ4bE3-40OKTv7ztKTILG3DlmJ9EI3uEfCrXiTOpLE5LbITOWU7N2WhXswichpsA5lehm-LCDSNIpfy7XJEG_YNsPn-4jWWpZ31ufoGKYUoLRBM_LN7VdTuh42UAY5wGIIUTF0A8EaQNtEw6ZCKTsMU91EVrWByDV0NfzRpkS&amp;xkcb=SoDT-_M3cgKcSUg5rj0IbzkdCdPP&amp;p=2&amp;fvj=0&amp;vjs=3</t>
+          <t>£4.40 an hour</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>test/rc/clk?jk=63779fc7e4e1e5f2&amp;fccid=905a967fd25ae49d&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Software Developer</t>
+          <t>Software Engineer Apprentice</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Arca Blanca</t>
+          <t>QA Apprenticeships</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>London</t>
+          <t>London TW8</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0DG4ntHtB_rMsnfhgmnSvK2brktLme1L4SiDeJjQ-izrVOLqRJ5-yjEhSyAj73O13RxN6ktcguadnTF--TVXDENJo5ZqCEoHBMTDiz68ennfSABB6NszvcA3cuxcUQYkELxKAtHBHdaxVaQ_TmpzFJQCZCR5DXVc3uIEvTcO9DcmZ9nig8PxjAiZuIkOe_4P_3_m5S48OB-UBORehDT6Ve4BJVdsWWoMMqcsRQJapP1STxYUfOX4zhMI8SARHoCF3aHf8LVg0TJM-Dmd9RdO9EZPdVkitadULe71JyORQEnU1Dp_QRlvkKM46G0afaLrIMEism5poyx2ByWxq-yDa-6qrza3E-iMrxTaRqU8DkD7UUVslHUm-S-5Qms3iEnWd5A52BQolHjiaXbG7-A0s2z4bQuSJCXr0Dyae17zL5nIc1LQr76Brd33oy9p2Ax11W3y56WP1k-h_3hOgws88ZzUvdSqW2EfUXfzwpWzA24ex575A3Pv7NxXSqBVPuQcq8PANzJrv40rPo-DNbC6iHEayz5TNhjgdm9vVPZz13EW9KqNX7YVP9mMdOVZ4UbMuakMGAmV8U1utVoudHZgpx3nSLRShN-47-JI-vDlhhem1GGLyvcFSL8R9Rj7TIpCv7Hazi30p5plljTNLvsumY235lGhQpAEahjc34oSOM3YJ2U3dXu0knlK9IQqCWL2X_EYaUcYd1qy9KPlH7NNRJ1oN88dJdFMFkmNfwAFhYlSDWj-IxNwlQPEaUHNaLX-GvyfbUL4YltwBp-Uy3D7-Sm0E3bNuQ9Ko0UeIQZvw4vQCXR72Ivu9A7ZAwTIc0wbU29H3qCS4ycGFsR9UfssjRQzrvAdyoNwWg3GqQe64jzbRCHHc43DqAqIlo_UEPFK_BYJXbZKfMmmPF5GdSQ5UhjRWRJgKzrwjj-IdXngLzVZI7-UVKa-jdCoYtDczkIVGsbdCGMgHHz2Kb1Oi2gMb3-&amp;xkcb=SoCj-_M3cgKcSXA5rj0KbzkdCdPP&amp;p=3&amp;fvj=0&amp;vjs=3</t>
+          <t>£20,000 a year</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>test/pagead/clk?mo=r&amp;ad=-6NYlbfkN0CXy9_N1TLC2ejqyTX_V4eQ4PmQ2039NyFlBjhJ2joCdiLJ2guK6p6gDxKa49r6zxjSg5XGI2hT26G5hch9mNuzoY5w7goGqmcNfC2DDEHXlsp8_Lo7x8TSxtXFBDW0VOlKt7Kf0mszN0utQPq0jsLsqgwtOPc52bi3BJrDqmGQyGnXwDlHBKqty8jiZnhuGBkJITRleNl6DU2WS2ckhTixJD0_K6DPaJyR6Y6Keb8EofWnAWcdbVKaOXK9XQ5quwPXVSK3GV3Bo_p-EjGFj77zsf0ZM4_Htg-mIqZBAKkPpl4BJMHcZXoUBKmwo15zCZjhrvw7JIxNcs_ARWI5bYBGp4s6BRM_E1CDdwSRBT6qslTWx2X7Knr4QqIPtOUavsz6kttv0XST2a2PEZ_Yt8mrhTRQjJEkaiXt85aUpzredDZs_g17PfWGJp0TgwNtSxugOifJf6ggvPznCl92EVSx2EtkwDzpDo2w2TGtHIiuFKrp3nx3iwaSNasT7oK7EmtX0f--CBVH15ztrOylAxJIYj-qCV2IXX7iddRhbvPdSTAdTpNOwBXp&amp;xkcb=SoAn-_M3c1NbXXQHsp0KbzkdCdPP&amp;p=6&amp;fvj=0&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Junior eCommerce Developer</t>
+          <t>Robotics Developer</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Charles Tyrwhitt</t>
+          <t>Barnet and Chase Farm Hospitals</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>London SW1A</t>
+          <t>London</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0DHfE158Vc_ztQfIyiV2G0das18a3e6jp_UBkP2IfDunIj3sI6ZYQ368lvpM14uJWBkAthdDMKCy2thE-1XDFGaiY3yGw1dAr5jyK_NyOLOcvNPfBMGIquGJbmjxp1HVAEo5UnNJp50EQ7ENzOeTFbKoj2U43tgyWmJlAsysVISksxnJkj0c8NXdqDUukChGbkHFEH_eR_B1wpMDbFucW3Z1UX7we6rGheOEE4PqRnE3PafFRODPmVD0yrv8VXTpwnyUYuH6vlzJWf7Ni7znnoXtYI5xEsLIX9qpwZpE4Wy5BBuc9yWGfOdtYDY6UfbrPGIoEF2RCnQ1xUknrwBH1uKLBpjRCPgoSV2ijoN4h86XFiOyzJ2azu2vEOvuljkfyUNE2qhC-wC12moM92w_PeZxbaOxkL5HX_gWACSm_-t8hxZPDDN3Leb3CRsQQGIK1-UdA2AGxWHZjPk3a8YWmTt2hnbQoeWRYCpS-44uBfdr_Ms_lWGyT5AZcHQN99m0M0fW5ZNhdxcVzb62iJb9suDRECI9cVXey9MHghIan1_vliI7iHXYt8L0hQ6DiXTTX_APQAG9L2eMaEqS7tfv7Le&amp;xkcb=SoCK-_M3cgKcSXA5rj0IbzkdCdPP&amp;p=4&amp;fvj=0&amp;vjs=3</t>
+          <t>£45,024 - £50,806 a year</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>test/rc/clk?jk=e897606392e83984&amp;fccid=7691ebb71b24124c&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Software Tester Apprentice - Test Engineer</t>
+          <t>Software Developer Veteran Training Programme</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Department for Work and Pensions</t>
+          <t>SaluteMyJob</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Hybrid remote in London</t>
+          <t>Woking</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://uk.indeed.com/rc/clk?jk=e93dac7d737a99b2&amp;fccid=bde86870b61ac61d&amp;vjs=3</t>
+          <t>£30,000 - £45,000 a year</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>test/company/SaluteMyJob/jobs/Software-Developer-Veteran-Training-Programme-2e5bfa9ee0f81f49?fccid=111f6b9664e56375&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Node.JS Software Developer</t>
+          <t>Software Support Engineer Degree Apprentice</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>KidsLoop</t>
+          <t>QA Apprenticeships</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>London</t>
+          <t>Weybridge KT13</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0DG4ntHtB_rMsnfhgmnSvK2brktLme1L4SiDeJjQ-izrVOLqRJ5-yjEhSyAj73O13RxN6ktcguadi_ZlJLGWu4rC6oogRdIW-NIIOUNUrodm3Tf_B9pv_RZMj20Ve92llCbAhbj6mWZ9JhYM5yMcIEMKie4oLbOUNK3CaZtm-0Z3uxyiMgI9j4ppkMC72gahCJnODMCgQQ3xM13-cbZhvn-B8tRPr6k90jdj-w8TdDfo29K28Alsz2gQ129x0y39C96AWU4eA1hR7PveXWwdQ5ii62g2zyrNF2mkiMOxXrKT83QTvxUeODUiFg1hx9J43ASzVyn2db-HSbfGrkvVODEOb4PwRCOFglLieRVOtLbkEz4NAWWt2At057DjO8A9CID84dr0HKSfFQmwM9eyfb8gxe5WixZlxSL4rLIVY6MyickEKj7GUP8V84QYbrQvaxhlpp-SH33Di-FgEvov1e8YG7blNswkUlZr2HfXHu8_F-2mhTAbhjuMXe6SksgIkLkMq5PvlKxJ8wxYLGEEYO3ulKt4dok5X4Lmxl5DOfXPsuYws5srZSKXF3q41xXZQSAjiz95xu9ZSRoSwYU6deeXWett4ab8BjqhqxDdHQ1qecocXDgUr8SCioqscrTZShJV5-VPn7BxuymFujIXZe2yscSzjAR4hIY-7zxARVugmHJpQvSxlbE7gT-US8OCSoIwUHHY5y2UUzbNQJY4x77lA6PGlQwsqg7YfyDxxz7y1-anf4XopVOT8YYqWvYXGQATznKLfPCWMqlzJY8YV1tYR-5iTuyOxjl2lRJM3T_mHXO0EDTcZIV0oicMuQs740t9x9pHD7blvIM8y5OMzIc-TMmQk9usCpLczdXM9k9kevF99rXHgUWkZWaSm2OBGH4sMH0LKatl9-H5IOXBEyZqzcFfHlPw0lzm7SV30_FsewL3zUxPmmCx58mDgo-HklHxDNXXK7F3e1T__m_AsGZ0uGYz8EXSVY=&amp;xkcb=SoBS-_M3cgKcSXg5rj0LbzkdCdPP&amp;p=6&amp;fvj=0&amp;vjs=3</t>
+          <t>£25,000 - £28,000 a year</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>test/pagead/clk?mo=r&amp;ad=-6NYlbfkN0CXy9_N1TLC2ejqyTX_V4eQ4PmQ2039NyFlBjhJ2joCdiLJ2guK6p6gDxKa49r6zxgiO854Ph9UtTNrnGuT_m6j4f4lvnPNlmnEtP0fthAefN3dVdqyYs1SAo_xq3EkMME-v2zAmZpURi2zEIn-tZnXw1K2iiPBVzrXrg_dOjKLAPekfv3DUM3izRKf3xk_KWgLNqczCkYih765V8AAhW8NCVCd-Ubq_Jftim8l-jq2VPQqoiBO9PWF7KGDhYj5_YIa6vzEY2Ff0R_8kTdX0x3DvKYQwHKkjBqg6CCmMUTQnZeF8xS4HcF42-YBOK44ALfKgZsR4M-mappq4kfG_9q3sZFaVth0BJWuG67-TpcUprGoSu6T69r4XRo-B_kiAyaD6_uqPj-vF43MycEEms-spPSb_hzwl97JTDnQChqOIsrcu7cmBep2kphAtu_z6Q4UhTEzqcFESzBo5XklwhVp1QGLGe2m15ce0kM7---tfJFKiewP-M3hRdzX92NHW2hs4juWcYJEtuzBQPfk3MuxwzAVMei40KQjfsaFctCahpCL4C0RVPsd&amp;xkcb=SoBY-_M3c1NbXWQHsp0LbzkdCdPP&amp;p=10&amp;fvj=0&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Junior JavaScript Developer</t>
+          <t>Programmer and Developer Apprentice</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Human Exponent Inc.</t>
+          <t>Penknife Integrated Marketing</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>London</t>
+          <t>Watford</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://uk.indeed.com/company/Human-Exponent-Inc./jobs/Junior-Javascript-Developer-4ffb29857e1ae5d0?fccid=b4757f25c14c2b76&amp;vjs=3</t>
+          <t>£10,000 - £12,000 a year</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>test/rc/clk?jk=7b8644857d4b5a7d&amp;fccid=1bbce0be4428fd2a&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Apprentice Software Developer</t>
+          <t>Software Development Teacher</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ITP</t>
+          <t>Big Creative Training Ltd</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>London W2</t>
+          <t>London</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://uk.indeed.com/company/Institute-of-Telecommunications-Professionals/jobs/Apprentice-Software-Developer-476684af9c3d2c1b?fccid=7658d045e2441b7a&amp;vjs=3</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Software Developer</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Ig Recruit Ltd</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Hybrid remote in London</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0DzFSXhtSQvn9oyRCOA6psFY_LWEYKJkh_kYNX4Ftteh7SDudwvmWFDGvVqCYY46KDuIXMvmGpvOr6r3eI6Efc9lqndbKp9fo_rOKkXQIhYoTVY4TvABX0Jy-aTsZ7_Zf65YHFmuCOe5wtM4FlyGIl-_mnDP-R2tcgrdgeXL0jh7SFjFLTK_WNNVO_zcX5VH5o1F1OaUihiFEe6wgnPTrp5Q9plHah9Z1hQ68wB4mv6URPohmlQBvobxsM8mWUvJ39ELjR4cnsZz25eLliliRMuiwTvHuUWB2_kl3NvbQpnphA8IBTU4FfySgktZHFDTFbeQYtPl4TWBCMLeP3qDxMPJM_QIgh-9KPyorrP86hMLyDNfp4xbLM2csd5_wemQI921RL90csCat44wXwVsUQ_umsTORLarBRb0F-GemEPfLRcR6WvufcCbiBJiQze8ik-zixXAAhPN4wJZpO29VlVl9mp0JIP9ooJw_YlAdVR3A==&amp;xkcb=SoDc-_M3cgKcSWA5rj0LbzkdCdPP&amp;p=9&amp;fvj=1&amp;vjs=3</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Software Developer</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>University College London Hospitals NHS Foundation...</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>London W1T</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>https://uk.indeed.com/rc/clk?jk=ba144bc39783b5d3&amp;fccid=2f6cf5b0f7c31d8e&amp;vjs=3</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Software Engineer, Apprenticeship</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Meta</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>London</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>https://uk.indeed.com/rc/clk?jk=6d672cb2de13bf92&amp;fccid=ba07516c418dda52&amp;vjs=3</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Apprentice Software Developer</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Softwire</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>London</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>https://uk.indeed.com/rc/clk?jk=e97c14fa64f87964&amp;fccid=ea94cafa08dade11&amp;vjs=3</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Angular Software Developer</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Cortex IT Recruitment</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Remote in London</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0B4I0z8Vg4C22bXJk453pUE2nnLCUOyY_R-ihB16RDW6wYQUKHhB-cMKfVt-iSg2CsIV8DUnuFgajp9QJEUR8yTGJCyqemjbWjrb5tHy7Xw3MUqZD6jqjW5DZHJu3N_Kc8Z_BALvrc2XFdSVbrIzBtleAflgHl8Q-0k0o-sl-uX1FRqEf1yCUzolWNBmt5YWLcgunI1DjmQqwIC9hVJM8HLbI8dm-FOsq0OPZn6gcQWEdDWbVFH4N38XGGZw0rhWJclCiNcYGiT0kvyrzt4IOmHQBTEs2q40jyDG6tlY9sFMjVBPKnhTZTXkARhIktgsiuDWe_Q2cSaZk0Y_6rvTMOlz5JR3raV7Q2ZnxtmyyXiJ1dw5XmoTgDi5A7EiW74VNmzgGVfEhAgoRJJaPdDHSmS3ufxEDILgmO277NeOdZEc_ZXYog19V68dpEkCDiWhVDX4sBa9W1NlToO5QUHzy1Jsra5gx_vpFDkdceP_pCytb0NYkr9_VcSK7NK4jlunDin3aj6LXSXiy62u2JJL6NoLNn3_O0GZo9xXwNKbqyd06aENxRw0dLFBh9S-eU7o-7Go5QOBgkLnW88Kk2MbyLPn9bRvnwD_svQ8HjIaUJ5ocdQEtu-kMvkUiPBFxXdmNlc37cQKDdQB-OontAor8RErP_fZxDoPGFXVDdaPD0n_1QmbyG3JZnji1ZoWAbnH8kEjbnOfV0pjDwbAZ-swSJ3wSh2POYOdjk=&amp;xkcb=SoAv-_M3cgKcSRA5rj0LbzkdCdPP&amp;p=13&amp;fvj=0&amp;vjs=3</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Junior Front End Web Developer</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Spectra Analytics</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>London SE1</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>https://uk.indeed.com/company/Spectra-Analytics/jobs/Junior-Front-End-Web-Developer-bb2012eef2ffcf55?fccid=a67149e619cddbac&amp;vjs=3</t>
+          <t>£27,000 - £33,000 a year</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>test/company/Big-Creative-Education---Apprenticeships/jobs/Software-Development-Teacher-34283d1df4002ff6?fccid=50ad3812a1dd6750&amp;vjs=3</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6"/>
+    <hyperlink ref="E8" r:id="rId7"/>
+    <hyperlink ref="E9" r:id="rId8"/>
+    <hyperlink ref="E10" r:id="rId9"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Now brings in more results however it's still a WIP
</commit_message>
<xml_diff>
--- a/jobs.xlsx
+++ b/jobs.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +49,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,27 +426,27 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Title</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Company</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Location</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Salary</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Apply Here</t>
         </is>
@@ -451,228 +455,228 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Associate Software Developer Apprentice</t>
+          <t>Junior Delphi Software Developer</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Pearson</t>
+          <t>Ernest Gordon Recruitment Limited</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Remote in London</t>
+          <t>Hybrid remote in London</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>£22,000 - £25,000 a year</t>
+          <t>£35,000 - £45,000 a year</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>test/rc/clk?jk=002bf4846fcb7d28&amp;fccid=915b1c0ee87e5e8a&amp;vjs=3</t>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0BLTG9DKC8iUEjzj5GMXRvbrRPPLtQ49bnVbnj2Qcpi6Ewh8amSvyViVIVvvK1NOl7hiZPohhxO-TdX8jV39FkrpMiK9C8hZHtRCo_dMV8m-p2n-XFYiC3dllN0JP0XV78w2aKlygOu8Tbp6vtiYlP0FYxu2E06YjHNJeNGnXwBLtLfXFzKiyUG4On-paPT3R0fFGp4885R6YOHVL6VCoOPvZsgf0dkc_KGWpNUD1h1m_IlNkkO4XNBSHvq7RrZeeHd_3lqTdopA74eDOiNzkoobvtrXaCWaAzuyqr1eT6XEKBsHq4TYdDx2gEKUHYCEI3I7NMNOKqy_Gt721sCw_pe4KMXdftxWPr3Qt-YCOJPh1vzXjt7yhWqoEUU4b15efPajehfur_Dx-hD-O56mhLToh1I7XIk8_8FHn3C3sI9tJGbN5eK2X2VXTxnnRKpq0CX4b7hjIlWkLy14Z7FBqGWZ_H-x8Jn-YrjxEZ6_RNq9nzlw8WQmVSnf45BWEFFHCAvd8a92hia10u8HS_mwJoB5vjws84CvtfA0T9GEes3ig==&amp;xkcb=SoAz-_M3bD5oxcRr0h0LbzkdCdPP&amp;p=0&amp;fvj=0&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Software Junior Developer Apprentice</t>
+          <t>Website Developer</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>QA Apprenticeships</t>
+          <t>Contra Agency</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>London EC2M</t>
+          <t>Temporarily Remote in London SE10</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>£25,000 - £30,000 a year</t>
+          <t>£40,586 - £45,175 a year</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>test/pagead/clk?mo=r&amp;ad=-6NYlbfkN0CXy9_N1TLC2ejqyTX_V4eQ4PmQ2039NyFlBjhJ2joCdiLJ2guK6p6gDxKa49r6zxjCTAdQ1uM6iXGzvNU-Yc7zz3hcZmLelAG_vJQZlpFH00o1s04wldLCcuG3xoLJUNvg5I_mfxXCc_PV8WtCkXK1fUnA5Ex_hentUerjmxq2xmbvt24wPEOhAt-4w0krKuY-5OC1YS1GG8ekoDS0pUvI9LB72Jbk-px0W1IHgYf2nnyKhygMNemCiNhxr6fwaA69LYKM45kVJZ45QUPOiGNyc0P3Bxd6RuqbJbi1M5HxoOAYwevuidoX8c1_R9ukVmVc48n3TDL0IMNmdc4N9vufm8IkpwGJZqwDrWj10JKh0p8tBBcpC2W2oaGSpfeBrtAhQTcwhgXFO7H2sMiaJ1SHql9Cg8qrSW8wW3OuRbyC9D1g_j8Y575urpomtH8gy-_h4m2_9wVcvLHsCr4CADU40sJAalV6IQXDY7FBh-hzlTmEi_TLXsHTyH5gt7ZglxClV7w7I8qPjXY0KCA00rNqdbwUZLvf0lypRVaTQDJk9tmrkLwVsDtJ&amp;xkcb=SoDK-_M3c1NbXUwHsp0LbzkdCdPP&amp;p=4&amp;fvj=0&amp;vjs=3</t>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0A9KeT3j6INblOOMK0U8DFhLDoyAsNib7P09fbwmcp215U8nGCR2aXBvcYy7emKlCjwtYDPafTJzoM0GdZoRmsPES45zwLju91ayXln_Su9KaR9f3S1X_CtHRqESpkdguRX5gpzzvhiKxQ__jj7N3YUzyOD_e4stmreX4HAgxICna5Keqb9l6VWOagWobUxPe5sapNEXR1XJ-IW_URhfNjEji7EIgKADnc_bSRwrL4818fNbb0zJU9OSTNYUrWg0fMfM1ux0oAblqHMUAtDz8OM2jkDmreu2fsw2YsKK73J1Zg0cajcE3TqN2juS177L3KJ0UYjoNwj079gxL2cVWflfmbmUEl4-8W4QA5Ze0puIx_at4ourBsqu89KHHz-cJ7Gp8Fdy8rYYi9eW-RxZ4cQ5_hUw6Cw3DWh4xGW2IxVh9_Uu84ZBI4R9hYL5Jm7Zr_X2DUWlKnQCHKCh4QUdwKTIijXtTUJzbcUz3TVfgb_2SrtI1I4pnhw&amp;xkcb=SoDC-_M3bD5oxcxr0h0KbzkdCdPP&amp;p=1&amp;fvj=1&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>We are recruiting an Apprentice Software Developer</t>
+          <t>Delphi Software Developer (Remote)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>thecitysecret</t>
+          <t>Ernest Gordon Recruitment Limited</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Remote in London</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>£4.40 an hour</t>
+          <t>£45,000 - £55,000 a year</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>test/rc/clk?jk=63779fc7e4e1e5f2&amp;fccid=905a967fd25ae49d&amp;vjs=3</t>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0BLTG9DKC8iUEjzj5GMXRvbrRPPLtQ49bnVbnj2Qcpi6Ewh8amSvyViVIVvvK1NOl5g0317UJAzIUtqgRtEvOQPB-t8BpmEIIPxQYPzV_yJckGzH2qz3vx6SLefP_uF1GrDOlOOLFBA5cdFc2haiyasTF4LforxBWUENCUX-XIR1Er1KBQV_xwxwJLt1GpKe4jgfx8Q8oHBguSVUO7xZ4xj3h6idzjnf8NuCykGlHPb0wzcjb96YwLnpqD_u2HtKJiFQ_YUceMtw6ZO8Gfr3JQv5CUktVknF8Yn8UlV9ajXLdGIeCvIaPYzMwiRXWm4cg5rqjKidGYJpVywn51m8ggE59cl_htWIE4zLtAnoEsQ6izEehH7RgF_rYZsoaromH-RkSm97KiW_XFDvZZxKq-gKoaq-jI9r6uHkIGQvJC4uL7xMnyxG2gedLcNbRMU5dQ7gtF7sGpfx253YqZ73YL_pLtYrlIVX-C5tRMsDPPNFwbsAZt1c1Yt06AGUEORDTbvp3Xa1I5i6Ee2TQj8RNeGxkrqDsoq_L6HZcpL_VzGqA==&amp;xkcb=SoAv-_M3bD5oxfRr0h0LbzkdCdPP&amp;p=3&amp;fvj=0&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Software Engineer Apprentice</t>
+          <t>Software Developer</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>QA Apprenticeships</t>
+          <t>Ig Recruit Ltd</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>London TW8</t>
+          <t>Hybrid remote in London</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>£20,000 a year</t>
+          <t>£45,000 - £70,000 a year</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>test/pagead/clk?mo=r&amp;ad=-6NYlbfkN0CXy9_N1TLC2ejqyTX_V4eQ4PmQ2039NyFlBjhJ2joCdiLJ2guK6p6gDxKa49r6zxjSg5XGI2hT26G5hch9mNuzoY5w7goGqmcNfC2DDEHXlsp8_Lo7x8TSxtXFBDW0VOlKt7Kf0mszN0utQPq0jsLsqgwtOPc52bi3BJrDqmGQyGnXwDlHBKqty8jiZnhuGBkJITRleNl6DU2WS2ckhTixJD0_K6DPaJyR6Y6Keb8EofWnAWcdbVKaOXK9XQ5quwPXVSK3GV3Bo_p-EjGFj77zsf0ZM4_Htg-mIqZBAKkPpl4BJMHcZXoUBKmwo15zCZjhrvw7JIxNcs_ARWI5bYBGp4s6BRM_E1CDdwSRBT6qslTWx2X7Knr4QqIPtOUavsz6kttv0XST2a2PEZ_Yt8mrhTRQjJEkaiXt85aUpzredDZs_g17PfWGJp0TgwNtSxugOifJf6ggvPznCl92EVSx2EtkwDzpDo2w2TGtHIiuFKrp3nx3iwaSNasT7oK7EmtX0f--CBVH15ztrOylAxJIYj-qCV2IXX7iddRhbvPdSTAdTpNOwBXp&amp;xkcb=SoAn-_M3c1NbXXQHsp0KbzkdCdPP&amp;p=6&amp;fvj=0&amp;vjs=3</t>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0DzFSXhtSQvn9oyRCOA6psFY_LWEYKJkh_kYNX4Ftteh7SDudwvmWFDGvVqCYY46KDuIXMvmGpvOr6r3eI6Efc9lqndbKp9fo_rOKkXQIhYoTVY4TvABX0Jy-aTsZ7_Zf65YHFmuCOe5wtM4FlyGIl-_mnDP-R2tcgrdgeXL0jh7e6QRiYc-IfyEtW78hINH3kkDACsI-GcVS-ZuXjtQjvHXChXLQkuHwgmC1lgYk47d0Xc6qUhDbWuBrYZTqbspRXf3sxD-f0DofM0UpM1qAwZcn8xWiHcWwRRuHz8CW8YXasYeCN3v0U8qcTwkEz-nZK7DdGyiICXMbIPuOI5cmlB_9Obc8G7fsWjz4hfmlkKssa0ycT4lUHEu5Btx8M5HLiRPBR9uphi3xxgJtSLKf_Pe_LZgFgFgJnWnUkP1Qai4afovvNtWDbkFVwbykwU_97N7yOWh9afus_o5ysIOa6MOKyxTj20Ocbqy98_0T8MjDVPxnaN__TT&amp;xkcb=SoAG-_M3bD5oxfRr0h0JbzkdCdPP&amp;p=4&amp;fvj=1&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Robotics Developer</t>
+          <t>Delphi Software Developer (Hybrid)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Barnet and Chase Farm Hospitals</t>
+          <t>Ernest Gordon Recruitment Limited</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>London</t>
+          <t>Hybrid remote in London</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>£45,024 - £50,806 a year</t>
+          <t>£45,000 - £55,000 a year</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>test/rc/clk?jk=e897606392e83984&amp;fccid=7691ebb71b24124c&amp;vjs=3</t>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0BLTG9DKC8iUEjzj5GMXRvbrRPPLtQ49bnVbnj2Qcpi6Ewh8amSvyViVIVvvK1NOl5g0317UJAzIVCybnQxMbOUNjV32AFxvix0wEt4hkIY9mdTYZDYXmsdjvA9lGOMl8m1smYKzECwACTNwQC-EHSWKuQ0iuBeIV2GlMjeyFe686gIyEXSxzxXX1VdITPf94HfIZAhQ0SxPNysNIpakdvGKwzGuKvjoO4CJgkc0poggDUjWrBy3bUKkwMlr-bm_23ZBw25tN27iq2F2-GgkkW1ty2eaKtOrTIokt8db6pYrslKzQ_I9WcIBLKBlmoK2L1rjr00Tm19DA0hY9JGutQVGjADCTgnYD2i03RKFkihdrc0PjJb-JuKElWbw15mgKej-wbAmW_wB4pxBgpZGv1v43nxKTFcdRiC-ZzZr1IxAgACZQBpJqWYJjvFGiCk-50b5XQt1NlmLgQ1CLpaXkDnBSP0vdCO0sAoe6qNCNXx7XYxfSxmiUpB9ZsNXOZOzomEi-j2xHXNjcw3mg_OR2KZHWL970xjf48=&amp;xkcb=SoBq-_M3bD5oxfxr0h0LbzkdCdPP&amp;p=5&amp;fvj=0&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Software Developer Veteran Training Programme</t>
+          <t>Graduate Delphi Software Developer</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>SaluteMyJob</t>
+          <t>Ernest Gordon Recruitment Limited</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Woking</t>
+          <t>Hybrid remote in London</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>£30,000 - £45,000 a year</t>
+          <t>£35,000 - £45,000 a year</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>test/company/SaluteMyJob/jobs/Software-Developer-Veteran-Training-Programme-2e5bfa9ee0f81f49?fccid=111f6b9664e56375&amp;vjs=3</t>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0BLTG9DKC8iUEjzj5GMXRvbrRPPLtQ49bnVbnj2Qcpi6Ewh8amSvyViVIVvvK1NOl7hiZPohhxO-S46WKZfQYYnhGZcpYpztB4Qipe9xy4-6DBJt5ytGu0Bxi0SSeCDkVO-cUXYb8e771fw1gDlm7K_xMyoPJwiCqhHYw7WW1zETPB_4ShCsL42eoiXCS2g95BMKyZdLrrNuEgJpEOTdQA45R7r7nzk07JFcUCrqUroXT3iZgC_GIGf4w1W2gXOk2EbZkbSpQHi_O4r-frdI6lbVcfr0mZqTjdlzy4BXRGJELw_hB31mZZ9WixvIWJC-0OfcDjoXjxToQ2KNiWC8WWgNFQ5PAZMi7aW387XK8NDflqywfxqNCHxBXfEfaCRUy4bqRJoAUdcWayjl8dnajVjuIgeJC7tLmBJSooYSaNyJi04E0iWyF9gh3XHkWlb8yLpv7FJF5elgXTT7v3nytywCJ36Jwcm6fwzeKO8Nb5WIEkSdCT93HWIKKzfV97KrZwO5rKr_8aESSjFXylijoLn98_kN6SZt3vdxHQCSd3x2KkhEVib0R__&amp;xkcb=SoBD-_M3bD5oxfxr0h0JbzkdCdPP&amp;p=7&amp;fvj=0&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Software Support Engineer Degree Apprentice</t>
+          <t>Software Developer - Your Return to Tech</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>QA Apprenticeships</t>
+          <t>Tech Returners</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Weybridge KT13</t>
+          <t>Temporarily Remote in London+2 locations</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>£25,000 - £28,000 a year</t>
+          <t>From £40,000 a year</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>test/pagead/clk?mo=r&amp;ad=-6NYlbfkN0CXy9_N1TLC2ejqyTX_V4eQ4PmQ2039NyFlBjhJ2joCdiLJ2guK6p6gDxKa49r6zxgiO854Ph9UtTNrnGuT_m6j4f4lvnPNlmnEtP0fthAefN3dVdqyYs1SAo_xq3EkMME-v2zAmZpURi2zEIn-tZnXw1K2iiPBVzrXrg_dOjKLAPekfv3DUM3izRKf3xk_KWgLNqczCkYih765V8AAhW8NCVCd-Ubq_Jftim8l-jq2VPQqoiBO9PWF7KGDhYj5_YIa6vzEY2Ff0R_8kTdX0x3DvKYQwHKkjBqg6CCmMUTQnZeF8xS4HcF42-YBOK44ALfKgZsR4M-mappq4kfG_9q3sZFaVth0BJWuG67-TpcUprGoSu6T69r4XRo-B_kiAyaD6_uqPj-vF43MycEEms-spPSb_hzwl97JTDnQChqOIsrcu7cmBep2kphAtu_z6Q4UhTEzqcFESzBo5XklwhVp1QGLGe2m15ce0kM7---tfJFKiewP-M3hRdzX92NHW2hs4juWcYJEtuzBQPfk3MuxwzAVMei40KQjfsaFctCahpCL4C0RVPsd&amp;xkcb=SoBY-_M3c1NbXWQHsp0LbzkdCdPP&amp;p=10&amp;fvj=0&amp;vjs=3</t>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0AbMsrYsAi0JFHPLu_2mW_2EIGQHZf3spZOFbDQNHXQWmYvxYTDL77sEfykw7oHF0h1biF3zRwYbwETm6-5cxbE0wfjxa-ZNT-YEhj8B9himkV_JNb6VuMpkmPsSqn2T0XJ3qSM0bkMfXhtxNiuWXf22Kcc88kzNWA8CEbLSt_IFrN3opWHgfjP3FxODISygU3Cbvg-LNeg1fvGpELzwVli5k9PVV_QZcVMLohx8CXDEFsLS8DUuRZELksGTYQubs-1YOMSes5HXPDmM4mAQWRhUZ1MhUgjnUSclkmcwB8uloGNTTxAjtvv9UGeNeWPJGel9JNk6ToiQPZBs7hFOnI1A-jjWozehZI6mfXOLfxeNrTgek_L1PA8MGktdftgeOBxlKgqTPPYSdbW1DuEpyoj_y0AvnMZEwL0UlPbuIoj6pMciTiiMRgM_ea-f22GaTkneXhoz34eGTkcecjBLB0Skst6zpQwyf4v4-hNs75o5EqRj0s_mM4OWtLoE7xprkGIDFIdiRS4Hg==&amp;xkcb=SoBQ-_M3bD5oxeRr0h0KbzkdCdPP&amp;p=8&amp;fvj=1&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Programmer and Developer Apprentice</t>
+          <t>Umbraco Developer - Fully Remote - £500+ per day - Outside I...</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Penknife Integrated Marketing</t>
+          <t>Edison Pope</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Watford</t>
+          <t>Remote in London</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>£10,000 - £12,000 a year</t>
+          <t>From £500 a day</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>test/rc/clk?jk=7b8644857d4b5a7d&amp;fccid=1bbce0be4428fd2a&amp;vjs=3</t>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0B62sP4HgT_bin6Q8ZuOedLyi0IXdvA6AE8k5EX4G5rP29lej8rB3Qex4moYYcYIbG1Z0Rg-2mE076IiCz8B8VfPWkv8uwOAvEBd1Q3qZvXQifJJh8okkaaA5M7y6XViUP1UEoGAQe3n20wEmrex6_YcCxbhfWoN39h7qfcwa6hjeCrS_AT-r1dAc2WE0IeHJcEylKfCft3IJeAi_pRh93pooTHsdizgIjhkfRmtCtw3trcSWpOjvyY4Ox26c00jViRzEc9KRiEZzLyOQZC-OX02hNUnLfM8Vr91k_7DmGjNTkhtZx0Y6jzjKJZyoO1EgtmGIFxTEBU4SiFeEjJYEttPgxp9iLZx0mAb4ZoZf80xo0E_Tl1O76EJKGRr5ULNoIwakpQiwLcyFnsfl4PvP_CPmcsRHLlgjAOtA5b4TfCtnAB3AciRQdNW_fzfmOdmRy1FEoR0C1RjmkYcAbaf8db1eZdnOUpEqcCT2A0m6YLftL1hmhQHyX1&amp;xkcb=SoB5-_M3bD5oxeRr0h0IbzkdCdPP&amp;p=9&amp;fvj=1&amp;vjs=3</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Software Development Teacher</t>
+          <t>Junior JavaScript Developer</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Big Creative Training Ltd</t>
+          <t>Human Exponent Inc.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -682,12 +686,93 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>£27,000 - £33,000 a year</t>
+          <t>£30,000 - £40,000 a year</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>test/company/Big-Creative-Education---Apprenticeships/jobs/Software-Development-Teacher-34283d1df4002ff6?fccid=50ad3812a1dd6750&amp;vjs=3</t>
+          <t>https://uk.indeed.com/company/Human-Exponent-Inc./jobs/Junior-Javascript-Developer-4ffb29857e1ae5d0?fccid=b4757f25c14c2b76&amp;vjs=3</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Software Developer Internship</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Inspiring Interns</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>£18,000 - £19,000 a year</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>https://uk.indeed.com/pagead/clk?mo=r&amp;ad=-6NYlbfkN0DzwreoEVFOkXRcFH1aYDKs9BsTnM4S4dXogYMNQuxRsWEvU3NmJBXmQipkwYVPqOyyWakXPnJku76CC3G11jOlJJl_Z-vD2e6CqEiCp4Xw5BmESzFcdir6NKaLvHdNE5m_HW0ROYcLmIm2F-BH_4hG_XB3HWa-WyT2T7s70oZyWPA5OdnFSdhBCOFQLiq8HX6O2PvWjintOy-bB3rwwWWHRitKYfS81uSFbsfQ1rv4XTjb4_YqfBwRyL8QHx0e00V9ydoge69SbNDyR9lI37fKetRQzFo080hexh9oJK14qcyfC_2ZFb3nZ7t6k13Tpk-W0we4BzLgH1S7bYlXmG0g28OtBS8YV0kDvJgghSSzCc17MURdMhfrvud_aBc2BViVMRY36VTmDeSIysca9pI_WWgqUiC-vk4yYkI7eh62x_NKLkdR4wkI3hg_qz9Ym-yzGM_MXAga4metIOJQq6OGmlse_Z4_eMb1mYGLh045mPHMHWgB2lsmIdpPeOxqVxU=&amp;xkcb=SoCh-_M3bD5oxexr0h0LbzkdCdPP&amp;p=11&amp;fvj=1&amp;vjs=3</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Software Development Internship</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Softwire</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>£28,000 a year</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>https://uk.indeed.com/rc/clk?jk=fc63bf03940b5708&amp;fccid=ea94cafa08dade11&amp;vjs=3</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Apprentice Software Developer</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Softwire</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>£24,000 a year</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>https://uk.indeed.com/rc/clk?jk=e97c14fa64f87964&amp;fccid=ea94cafa08dade11&amp;vjs=3</t>
         </is>
       </c>
     </row>
@@ -702,6 +787,9 @@
     <hyperlink ref="E8" r:id="rId7"/>
     <hyperlink ref="E9" r:id="rId8"/>
     <hyperlink ref="E10" r:id="rId9"/>
+    <hyperlink ref="E11" r:id="rId10"/>
+    <hyperlink ref="E12" r:id="rId11"/>
+    <hyperlink ref="E13" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>